<commit_message>
Reacomodacion de balances, aun deficiente.
</commit_message>
<xml_diff>
--- a/datos/filas_y_columnas_balances.xlsx
+++ b/datos/filas_y_columnas_balances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renato\GitHub\scn_gt\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573B9EA4-3B96-41C5-8761-E6683C79B915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C8767B-01A7-47BF-BBB2-53BDBA131373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6CAF9067-E9DD-4BAA-A4C4-ED4C1F61F977}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="1" xr2:uid="{6CAF9067-E9DD-4BAA-A4C4-ED4C1F61F977}"/>
   </bookViews>
   <sheets>
     <sheet name="filas" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="174">
   <si>
     <t>OFERTA TOTAL</t>
   </si>
@@ -558,9 +558,6 @@
   </si>
   <si>
     <t>Utilización</t>
-  </si>
-  <si>
-    <t>No aplica</t>
   </si>
 </sst>
 </file>
@@ -942,21 +939,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7235EAF2-435C-47D5-BA9B-1EA106F44974}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.53515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.23046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -979,7 +976,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1002,7 +999,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1025,7 +1022,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1048,7 +1045,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1071,7 +1068,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1094,7 +1091,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1117,7 +1114,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1134,13 +1131,13 @@
         <v>73</v>
       </c>
       <c r="F8" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1157,13 +1154,13 @@
         <v>74</v>
       </c>
       <c r="F9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1180,13 +1177,13 @@
         <v>75</v>
       </c>
       <c r="F10" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1203,13 +1200,13 @@
         <v>76</v>
       </c>
       <c r="F11" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1226,13 +1223,13 @@
         <v>77</v>
       </c>
       <c r="F12" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1249,13 +1246,13 @@
         <v>78</v>
       </c>
       <c r="F13" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1272,13 +1269,13 @@
         <v>79</v>
       </c>
       <c r="F14" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1295,13 +1292,13 @@
         <v>80</v>
       </c>
       <c r="F15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1318,13 +1315,13 @@
         <v>81</v>
       </c>
       <c r="F16" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -1341,13 +1338,13 @@
         <v>82</v>
       </c>
       <c r="F17" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1364,13 +1361,13 @@
         <v>83</v>
       </c>
       <c r="F18" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1387,13 +1384,13 @@
         <v>84</v>
       </c>
       <c r="F19" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -1416,7 +1413,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
@@ -1439,7 +1436,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
@@ -1462,7 +1459,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
@@ -1485,7 +1482,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
@@ -1508,7 +1505,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
@@ -1531,7 +1528,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
@@ -1554,7 +1551,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
@@ -1577,7 +1574,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
@@ -1610,20 +1607,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A871C8D-2B72-4908-8864-4A4A6020CCC3}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.07421875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>140</v>
       </c>
@@ -1640,7 +1637,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -1657,7 +1654,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>118</v>
       </c>
@@ -1674,7 +1671,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>119</v>
       </c>
@@ -1691,7 +1688,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>120</v>
       </c>
@@ -1708,7 +1705,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>121</v>
       </c>
@@ -1725,7 +1722,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>122</v>
       </c>
@@ -1742,7 +1739,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>123</v>
       </c>
@@ -1759,7 +1756,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>124</v>
       </c>
@@ -1776,7 +1773,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
@@ -1793,7 +1790,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>126</v>
       </c>
@@ -1810,7 +1807,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>127</v>
       </c>
@@ -1827,7 +1824,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>128</v>
       </c>
@@ -1844,7 +1841,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>129</v>
       </c>
@@ -1861,7 +1858,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>130</v>
       </c>
@@ -1878,7 +1875,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>131</v>
       </c>
@@ -1895,7 +1892,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>132</v>
       </c>
@@ -1912,7 +1909,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>133</v>
       </c>
@@ -1929,7 +1926,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>134</v>
       </c>
@@ -1946,7 +1943,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>135</v>
       </c>
@@ -1963,7 +1960,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>136</v>
       </c>
@@ -1980,7 +1977,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>137</v>
       </c>
@@ -1997,7 +1994,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>138</v>
       </c>
@@ -2014,7 +2011,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>139</v>
       </c>

</xml_diff>

<commit_message>
Se realizaron cambios de signo y concepto para que la oferta este en balance con la utilizacion.
</commit_message>
<xml_diff>
--- a/datos/filas_y_columnas_balances.xlsx
+++ b/datos/filas_y_columnas_balances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renato\GitHub\scn_gt\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C8767B-01A7-47BF-BBB2-53BDBA131373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC1E132-3AFB-4C3D-ABC1-F104A41649B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="1" xr2:uid="{6CAF9067-E9DD-4BAA-A4C4-ED4C1F61F977}"/>
+    <workbookView xWindow="3797" yWindow="2983" windowWidth="15849" windowHeight="8966" activeTab="1" xr2:uid="{6CAF9067-E9DD-4BAA-A4C4-ED4C1F61F977}"/>
   </bookViews>
   <sheets>
     <sheet name="filas" sheetId="1" r:id="rId1"/>
@@ -356,12 +356,6 @@
     <t>Gas Licuado De Petróleo</t>
   </si>
   <si>
-    <t>Gasolina/Alcohol</t>
-  </si>
-  <si>
-    <t>Kerosene/Jet Fuel</t>
-  </si>
-  <si>
     <t>Diésel Oil</t>
   </si>
   <si>
@@ -558,6 +552,12 @@
   </si>
   <si>
     <t>Utilización</t>
+  </si>
+  <si>
+    <t>Gasolina / Alcohol</t>
+  </si>
+  <si>
+    <t>Kerosene / Jet Fuel</t>
   </si>
 </sst>
 </file>
@@ -940,17 +940,21 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="1" width="13.84375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.53515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.23046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.07421875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.23046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.3828125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
@@ -970,10 +974,10 @@
         <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -996,7 +1000,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
@@ -1019,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
@@ -1042,7 +1046,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -1065,7 +1069,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -1088,7 +1092,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
@@ -1111,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
@@ -1134,7 +1138,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -1157,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -1180,7 +1184,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
@@ -1203,7 +1207,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
@@ -1226,7 +1230,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
@@ -1249,7 +1253,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
@@ -1272,7 +1276,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
@@ -1295,7 +1299,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
@@ -1318,7 +1322,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
@@ -1341,7 +1345,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
@@ -1364,7 +1368,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
@@ -1387,7 +1391,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
@@ -1410,7 +1414,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
@@ -1433,7 +1437,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
@@ -1456,7 +1460,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
@@ -1479,7 +1483,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
@@ -1502,7 +1506,7 @@
         <v>2</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
@@ -1525,7 +1529,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
@@ -1548,7 +1552,7 @@
         <v>2</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
@@ -1571,7 +1575,7 @@
         <v>2</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
@@ -1594,7 +1598,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1608,7 +1612,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1622,33 +1626,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>94</v>
@@ -1656,16 +1660,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>95</v>
@@ -1673,16 +1677,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>96</v>
@@ -1690,16 +1694,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>97</v>
@@ -1707,16 +1711,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>98</v>
@@ -1724,16 +1728,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>99</v>
@@ -1741,16 +1745,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>100</v>
@@ -1758,16 +1762,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>101</v>
@@ -1775,16 +1779,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>102</v>
@@ -1792,16 +1796,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>103</v>
@@ -1809,16 +1813,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B12" s="2">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>104</v>
@@ -1826,16 +1830,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>105</v>
@@ -1843,189 +1847,189 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B14" s="2">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>106</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>107</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B17" s="2">
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B18" s="2">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B19" s="2">
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B21" s="2">
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B22" s="2">
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B23" s="2">
         <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B24" s="2">
         <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>